<commit_message>
Flyback çalıştı !!!! Fanlar döndü. 220V'ta patladı. Hata tespit edildi ama entegremiz yok :)
</commit_message>
<xml_diff>
--- a/Prototype/Test/kontrol kartı/ControlPower.xlsx
+++ b/Prototype/Test/kontrol kartı/ControlPower.xlsx
@@ -2371,8 +2371,8 @@
   </sheetPr>
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>